<commit_message>
Adicionado mineração das análises
</commit_message>
<xml_diff>
--- a/Análises.xlsx
+++ b/Análises.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rodrigo\Google Drive\7º semestre\IA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rodrigo\Google Drive\7º semestre\IA\Genetics\AlgoritimosGeneticosIA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="36">
   <si>
     <t>Número do teste</t>
   </si>
@@ -58,66 +58,6 @@
     <t>Simulação 01</t>
   </si>
   <si>
-    <t>Ciclo 20</t>
-  </si>
-  <si>
-    <t>Ciclo 19</t>
-  </si>
-  <si>
-    <t>Ciclo 18</t>
-  </si>
-  <si>
-    <t>Ciclo 17</t>
-  </si>
-  <si>
-    <t>Ciclo 16</t>
-  </si>
-  <si>
-    <t>Ciclo 15</t>
-  </si>
-  <si>
-    <t>Ciclo 14</t>
-  </si>
-  <si>
-    <t>Ciclo 13</t>
-  </si>
-  <si>
-    <t>Ciclo 12</t>
-  </si>
-  <si>
-    <t>Ciclo 11</t>
-  </si>
-  <si>
-    <t>Ciclo 10</t>
-  </si>
-  <si>
-    <t>Ciclo 9</t>
-  </si>
-  <si>
-    <t>Ciclo 8</t>
-  </si>
-  <si>
-    <t>Ciclo 7</t>
-  </si>
-  <si>
-    <t>Ciclo 6</t>
-  </si>
-  <si>
-    <t>Ciclo 5</t>
-  </si>
-  <si>
-    <t>Ciclo 4</t>
-  </si>
-  <si>
-    <t>Ciclo 3</t>
-  </si>
-  <si>
-    <t>Ciclo 2</t>
-  </si>
-  <si>
-    <t>Ciclo 1</t>
-  </si>
-  <si>
     <t xml:space="preserve">100 ciclos com 80 % da população inicial que era de 11 individuos  </t>
   </si>
   <si>
@@ -131,6 +71,69 @@
   </si>
   <si>
     <t xml:space="preserve">50 ciclos com 40 % da população inicial que era de 11 individuos  </t>
+  </si>
+  <si>
+    <t>200 ciclos, 80% da população, entrada 11</t>
+  </si>
+  <si>
+    <t>Amostra 1</t>
+  </si>
+  <si>
+    <t>Amostra 2</t>
+  </si>
+  <si>
+    <t>Amostra 3</t>
+  </si>
+  <si>
+    <t>Amostra 4</t>
+  </si>
+  <si>
+    <t>Amostra 5</t>
+  </si>
+  <si>
+    <t>Amostra 6</t>
+  </si>
+  <si>
+    <t>Amostra 7</t>
+  </si>
+  <si>
+    <t>Amostra 8</t>
+  </si>
+  <si>
+    <t>Amostra 9</t>
+  </si>
+  <si>
+    <t>Amostra 10</t>
+  </si>
+  <si>
+    <t>Amostra 11</t>
+  </si>
+  <si>
+    <t>Amostra 12</t>
+  </si>
+  <si>
+    <t>Amostra 13</t>
+  </si>
+  <si>
+    <t>Amostra 14</t>
+  </si>
+  <si>
+    <t>Amostra 15</t>
+  </si>
+  <si>
+    <t>Amostra 16</t>
+  </si>
+  <si>
+    <t>Amostra 17</t>
+  </si>
+  <si>
+    <t>Amostra 18</t>
+  </si>
+  <si>
+    <t>Amostra 19</t>
+  </si>
+  <si>
+    <t>Amostra 20</t>
   </si>
 </sst>
 </file>
@@ -168,7 +171,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -219,8 +222,13 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -239,8 +247,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="10">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -251,28 +274,33 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="9"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="8" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="6" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="9"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="8" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="10" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="10" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="10">
+  <cellStyles count="11">
     <cellStyle name="40% - Ênfase1" xfId="3" builtinId="31"/>
     <cellStyle name="40% - Ênfase2" xfId="5" builtinId="35"/>
     <cellStyle name="40% - Ênfase3" xfId="7" builtinId="39"/>
@@ -282,6 +310,7 @@
     <cellStyle name="Ênfase3" xfId="6" builtinId="37"/>
     <cellStyle name="Ênfase6" xfId="8" builtinId="49"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Nota" xfId="10" builtinId="10"/>
     <cellStyle name="Total" xfId="1" builtinId="25"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -727,11 +756,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="174174512"/>
-        <c:axId val="174176080"/>
+        <c:axId val="320616664"/>
+        <c:axId val="320614312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="174174512"/>
+        <c:axId val="320616664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -774,7 +803,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="174176080"/>
+        <c:crossAx val="320614312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -782,7 +811,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="174176080"/>
+        <c:axId val="320614312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="44"/>
@@ -849,7 +878,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="174174512"/>
+        <c:crossAx val="320616664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -1349,11 +1378,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="240243240"/>
-        <c:axId val="240242064"/>
+        <c:axId val="322314936"/>
+        <c:axId val="322316504"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="240243240"/>
+        <c:axId val="322314936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1396,7 +1425,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="240242064"/>
+        <c:crossAx val="322316504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1404,7 +1433,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="240242064"/>
+        <c:axId val="322316504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1455,7 +1484,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="240243240"/>
+        <c:crossAx val="322314936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1622,7 +1651,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Ciclo 1</c:v>
+                  <c:v>Amostra 1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1752,7 +1781,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Ciclo 2</c:v>
+                  <c:v>Amostra 2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1882,7 +1911,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Ciclo 3</c:v>
+                  <c:v>Amostra 3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2012,7 +2041,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Ciclo 4</c:v>
+                  <c:v>Amostra 4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2142,7 +2171,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Ciclo 5</c:v>
+                  <c:v>Amostra 5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2272,7 +2301,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Ciclo 6</c:v>
+                  <c:v>Amostra 6</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2402,7 +2431,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Ciclo 7</c:v>
+                  <c:v>Amostra 7</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2534,7 +2563,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Ciclo 8</c:v>
+                  <c:v>Amostra 8</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2666,7 +2695,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Ciclo 9</c:v>
+                  <c:v>Amostra 9</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2798,7 +2827,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Ciclo 10</c:v>
+                  <c:v>Amostra 10</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2930,7 +2959,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Ciclo 11</c:v>
+                  <c:v>Amostra 11</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3062,7 +3091,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Ciclo 12</c:v>
+                  <c:v>Amostra 12</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3194,7 +3223,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Ciclo 13</c:v>
+                  <c:v>Amostra 13</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3327,7 +3356,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Ciclo 14</c:v>
+                  <c:v>Amostra 14</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3460,7 +3489,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Ciclo 15</c:v>
+                  <c:v>Amostra 15</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3593,7 +3622,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Ciclo 16</c:v>
+                  <c:v>Amostra 16</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3726,7 +3755,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Ciclo 17</c:v>
+                  <c:v>Amostra 17</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3859,7 +3888,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Ciclo 18</c:v>
+                  <c:v>Amostra 18</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3992,7 +4021,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Ciclo 19</c:v>
+                  <c:v>Amostra 19</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4124,7 +4153,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Ciclo 20</c:v>
+                  <c:v>Amostra 20</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4258,11 +4287,11 @@
         </c:dLbls>
         <c:gapWidth val="444"/>
         <c:overlap val="-90"/>
-        <c:axId val="598621192"/>
-        <c:axId val="598627072"/>
+        <c:axId val="322317288"/>
+        <c:axId val="320610000"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="598621192"/>
+        <c:axId val="322317288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4319,7 +4348,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="598627072"/>
+        <c:crossAx val="320610000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4327,7 +4356,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="598627072"/>
+        <c:axId val="320610000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="45"/>
@@ -4339,7 +4368,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="598621192"/>
+        <c:crossAx val="322317288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4852,11 +4881,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="174792976"/>
-        <c:axId val="174793368"/>
+        <c:axId val="320616272"/>
+        <c:axId val="320614704"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="174792976"/>
+        <c:axId val="320616272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4899,7 +4928,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="174793368"/>
+        <c:crossAx val="320614704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4907,7 +4936,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="174793368"/>
+        <c:axId val="320614704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="3.5000000000000003E-2"/>
@@ -4959,7 +4988,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="174792976"/>
+        <c:crossAx val="320616272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5145,7 +5174,9 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -5466,11 +5497,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="221798024"/>
-        <c:axId val="224236336"/>
+        <c:axId val="320615488"/>
+        <c:axId val="320609216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="221798024"/>
+        <c:axId val="320615488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5513,7 +5544,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="224236336"/>
+        <c:crossAx val="320609216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5521,7 +5552,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="224236336"/>
+        <c:axId val="320609216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="34"/>
@@ -5573,7 +5604,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="221798024"/>
+        <c:crossAx val="320615488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6103,11 +6134,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="224231632"/>
-        <c:axId val="224231240"/>
+        <c:axId val="320611176"/>
+        <c:axId val="320611960"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="224231632"/>
+        <c:axId val="320611176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6150,7 +6181,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="224231240"/>
+        <c:crossAx val="320611960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6158,7 +6189,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="224231240"/>
+        <c:axId val="320611960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="3.5000000000000003E-2"/>
@@ -6210,7 +6241,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="224231632"/>
+        <c:crossAx val="320611176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6719,11 +6750,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="224233200"/>
-        <c:axId val="224228888"/>
+        <c:axId val="322313368"/>
+        <c:axId val="322317680"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="224233200"/>
+        <c:axId val="322313368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6766,7 +6797,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="224228888"/>
+        <c:crossAx val="322317680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6774,7 +6805,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="224228888"/>
+        <c:axId val="322317680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6825,7 +6856,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="224233200"/>
+        <c:crossAx val="322313368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7324,11 +7355,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="224229672"/>
-        <c:axId val="224230064"/>
+        <c:axId val="322315328"/>
+        <c:axId val="322311016"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="224229672"/>
+        <c:axId val="322315328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7371,7 +7402,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="224230064"/>
+        <c:crossAx val="322311016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7379,7 +7410,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="224230064"/>
+        <c:axId val="322311016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7430,7 +7461,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="224229672"/>
+        <c:crossAx val="322315328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7933,11 +7964,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="224234376"/>
-        <c:axId val="224234768"/>
+        <c:axId val="322315720"/>
+        <c:axId val="322312976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="224234376"/>
+        <c:axId val="322315720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7980,7 +8011,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="224234768"/>
+        <c:crossAx val="322312976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7988,7 +8019,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="224234768"/>
+        <c:axId val="322312976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="37"/>
@@ -8040,7 +8071,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="224234376"/>
+        <c:crossAx val="322315720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8547,11 +8578,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="224235552"/>
-        <c:axId val="240244024"/>
+        <c:axId val="322311408"/>
+        <c:axId val="322313760"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="224235552"/>
+        <c:axId val="322311408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8594,7 +8625,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="240244024"/>
+        <c:crossAx val="322313760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8602,7 +8633,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="240244024"/>
+        <c:axId val="322313760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="8.8000000000000023E-2"/>
@@ -8669,7 +8700,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="224235552"/>
+        <c:crossAx val="322311408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9175,11 +9206,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="240244416"/>
-        <c:axId val="240246768"/>
+        <c:axId val="322314152"/>
+        <c:axId val="322312192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="240244416"/>
+        <c:axId val="322314152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9222,7 +9253,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="240246768"/>
+        <c:crossAx val="322312192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9230,7 +9261,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="240246768"/>
+        <c:axId val="322312192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="37"/>
@@ -9282,7 +9313,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="240244416"/>
+        <c:crossAx val="322314152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15612,15 +15643,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>462241</xdr:colOff>
+      <xdr:colOff>462240</xdr:colOff>
       <xdr:row>80</xdr:row>
       <xdr:rowOff>178734</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>276224</xdr:colOff>
-      <xdr:row>96</xdr:row>
-      <xdr:rowOff>66676</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15642,15 +15673,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>593912</xdr:colOff>
+      <xdr:colOff>12887</xdr:colOff>
       <xdr:row>81</xdr:row>
-      <xdr:rowOff>1119</xdr:rowOff>
+      <xdr:rowOff>10644</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>95</xdr:row>
-      <xdr:rowOff>104774</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15739,13 +15770,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>357187</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:rowOff>185736</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15772,10 +15803,10 @@
       <xdr:rowOff>157162</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15802,15 +15833,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>876300</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:colOff>819150</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>4764</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>52390</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>557214</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>185740</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -16100,7 +16131,7 @@
   <dimension ref="B2:L79"/>
   <sheetViews>
     <sheetView topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U93" sqref="U93"/>
+      <selection activeCell="X94" sqref="X94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16109,242 +16140,242 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
+      <c r="B2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="5">
         <v>1</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="5">
         <v>2</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="5">
         <v>3</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="5">
         <v>4</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="5">
         <v>5</v>
       </c>
-      <c r="H3" s="8">
+      <c r="H3" s="5">
         <v>6</v>
       </c>
-      <c r="I3" s="8">
+      <c r="I3" s="5">
         <v>7</v>
       </c>
-      <c r="J3" s="8">
+      <c r="J3" s="5">
         <v>8</v>
       </c>
-      <c r="K3" s="8">
+      <c r="K3" s="5">
         <v>9</v>
       </c>
-      <c r="L3" s="8">
+      <c r="L3" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="5">
         <v>41</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="5">
         <v>43</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="5">
         <v>41</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="5">
         <v>41</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="5">
         <v>42</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="5">
         <v>40</v>
       </c>
-      <c r="I4" s="8">
+      <c r="I4" s="5">
         <v>39</v>
       </c>
-      <c r="J4" s="8">
+      <c r="J4" s="5">
         <v>38</v>
       </c>
-      <c r="K4" s="8">
+      <c r="K4" s="5">
         <v>38</v>
       </c>
-      <c r="L4" s="8">
+      <c r="L4" s="5">
         <v>38</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="5">
         <v>0.06</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="5">
         <v>0.04</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="5">
         <v>0.06</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="5">
         <v>0.06</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="5">
         <v>0.05</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H5" s="5">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="I5" s="8">
+      <c r="I5" s="5">
         <v>0.08</v>
       </c>
-      <c r="J5" s="8">
+      <c r="J5" s="5">
         <v>0.09</v>
       </c>
-      <c r="K5" s="8">
+      <c r="K5" s="5">
         <v>0.09</v>
       </c>
-      <c r="L5" s="8">
+      <c r="L5" s="5">
         <v>0.09</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="5">
         <f>SUM(C4:L4)/10</f>
         <v>40.1</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="5">
         <f>SUM(C4:L4)/10</f>
         <v>40.1</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="5">
         <f>SUM(C4:L4)/10</f>
         <v>40.1</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="5">
         <f>SUM(C4:L4)/10</f>
         <v>40.1</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="5">
         <f>SUM(C4:L4)/10</f>
         <v>40.1</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="5">
         <f>SUM(C4:L4)/10</f>
         <v>40.1</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I7" s="5">
         <f>SUM(C4:L4)/10</f>
         <v>40.1</v>
       </c>
-      <c r="J7" s="8">
+      <c r="J7" s="5">
         <f>SUM(C4:L4)/10</f>
         <v>40.1</v>
       </c>
-      <c r="K7" s="8">
+      <c r="K7" s="5">
         <f>SUM(C4:L4)/10</f>
         <v>40.1</v>
       </c>
-      <c r="L7" s="8">
+      <c r="L7" s="5">
         <f>SUM(C4:L4)/10</f>
         <v>40.1</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="5">
         <f>SUM(C5:L5)/10</f>
         <v>6.8999999999999992E-2</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="5">
         <f>SUM(C5:L5)/10</f>
         <v>6.8999999999999992E-2</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="5">
         <f>SUM(C5:L5)/10</f>
         <v>6.8999999999999992E-2</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="5">
         <f>SUM(C5:L5)/10</f>
         <v>6.8999999999999992E-2</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="5">
         <f>SUM(C5:L5)/10</f>
         <v>6.8999999999999992E-2</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="5">
         <f>SUM(C5:L5)/10</f>
         <v>6.8999999999999992E-2</v>
       </c>
-      <c r="I8" s="8">
+      <c r="I8" s="5">
         <f>SUM(C5:L5)/10</f>
         <v>6.8999999999999992E-2</v>
       </c>
-      <c r="J8" s="8">
+      <c r="J8" s="5">
         <f>SUM(C5:L5)/10</f>
         <v>6.8999999999999992E-2</v>
       </c>
-      <c r="K8" s="8">
+      <c r="K8" s="5">
         <f>SUM(C5:L5)/10</f>
         <v>6.8999999999999992E-2</v>
       </c>
-      <c r="L8" s="8">
+      <c r="L8" s="5">
         <f>SUM(C5:L5)/10</f>
         <v>6.8999999999999992E-2</v>
       </c>
     </row>
     <row r="40" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B40" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
-      <c r="I40" s="3"/>
-      <c r="J40" s="3"/>
-      <c r="K40" s="3"/>
-      <c r="L40" s="3"/>
+      <c r="B40" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="7"/>
+      <c r="K40" s="7"/>
+      <c r="L40" s="7"/>
     </row>
     <row r="41" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
@@ -16555,224 +16586,224 @@
       </c>
     </row>
     <row r="73" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B73" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C73" s="6"/>
-      <c r="D73" s="6"/>
-      <c r="E73" s="6"/>
-      <c r="F73" s="6"/>
-      <c r="G73" s="6"/>
-      <c r="H73" s="6"/>
-      <c r="I73" s="6"/>
-      <c r="J73" s="6"/>
-      <c r="K73" s="6"/>
-      <c r="L73" s="6"/>
+      <c r="B73" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C73" s="8"/>
+      <c r="D73" s="8"/>
+      <c r="E73" s="8"/>
+      <c r="F73" s="8"/>
+      <c r="G73" s="8"/>
+      <c r="H73" s="8"/>
+      <c r="I73" s="8"/>
+      <c r="J73" s="8"/>
+      <c r="K73" s="8"/>
+      <c r="L73" s="8"/>
     </row>
     <row r="74" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B74" s="5" t="s">
+      <c r="B74" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C74" s="5">
+      <c r="C74" s="4">
         <v>1</v>
       </c>
-      <c r="D74" s="5">
+      <c r="D74" s="4">
         <v>2</v>
       </c>
-      <c r="E74" s="5">
+      <c r="E74" s="4">
         <v>3</v>
       </c>
-      <c r="F74" s="5">
+      <c r="F74" s="4">
         <v>4</v>
       </c>
-      <c r="G74" s="5">
+      <c r="G74" s="4">
         <v>5</v>
       </c>
-      <c r="H74" s="5">
+      <c r="H74" s="4">
         <v>6</v>
       </c>
-      <c r="I74" s="5">
+      <c r="I74" s="4">
         <v>7</v>
       </c>
-      <c r="J74" s="5">
+      <c r="J74" s="4">
         <v>8</v>
       </c>
-      <c r="K74" s="5">
+      <c r="K74" s="4">
         <v>9</v>
       </c>
-      <c r="L74" s="5">
+      <c r="L74" s="4">
         <v>10</v>
       </c>
     </row>
     <row r="75" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B75" s="5" t="s">
+      <c r="B75" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C75" s="5">
+      <c r="C75" s="4">
         <v>33</v>
       </c>
-      <c r="D75" s="5">
+      <c r="D75" s="4">
         <v>34</v>
       </c>
-      <c r="E75" s="5">
+      <c r="E75" s="4">
         <v>34</v>
       </c>
-      <c r="F75" s="5">
+      <c r="F75" s="4">
         <v>32</v>
       </c>
-      <c r="G75" s="5">
+      <c r="G75" s="4">
         <v>34</v>
       </c>
-      <c r="H75" s="5">
+      <c r="H75" s="4">
         <v>34</v>
       </c>
-      <c r="I75" s="5">
+      <c r="I75" s="4">
         <v>34</v>
       </c>
-      <c r="J75" s="5">
+      <c r="J75" s="4">
         <v>34</v>
       </c>
-      <c r="K75" s="5">
+      <c r="K75" s="4">
         <v>34</v>
       </c>
-      <c r="L75" s="5">
+      <c r="L75" s="4">
         <v>32</v>
       </c>
     </row>
     <row r="76" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B76" s="5" t="s">
+      <c r="B76" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C76" s="5">
+      <c r="C76" s="4">
         <v>0.36699999999999999</v>
       </c>
-      <c r="D76" s="5">
+      <c r="D76" s="4">
         <v>0.03</v>
       </c>
-      <c r="E76" s="5">
+      <c r="E76" s="4">
         <v>0.03</v>
       </c>
-      <c r="F76" s="5">
+      <c r="F76" s="4">
         <v>0.04</v>
       </c>
-      <c r="G76" s="5">
+      <c r="G76" s="4">
         <v>0.03</v>
       </c>
-      <c r="H76" s="5">
+      <c r="H76" s="4">
         <v>0.03</v>
       </c>
-      <c r="I76" s="5">
+      <c r="I76" s="4">
         <v>0.03</v>
       </c>
-      <c r="J76" s="5">
+      <c r="J76" s="4">
         <v>0.03</v>
       </c>
-      <c r="K76" s="5">
+      <c r="K76" s="4">
         <v>0.03</v>
       </c>
-      <c r="L76" s="5">
+      <c r="L76" s="4">
         <v>0.03</v>
       </c>
     </row>
     <row r="77" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B77" s="5"/>
-      <c r="C77" s="5"/>
-      <c r="D77" s="5"/>
-      <c r="E77" s="5"/>
-      <c r="F77" s="5"/>
-      <c r="G77" s="5"/>
-      <c r="H77" s="5"/>
-      <c r="I77" s="5"/>
-      <c r="J77" s="5"/>
-      <c r="K77" s="5"/>
-      <c r="L77" s="5"/>
+      <c r="B77" s="4"/>
+      <c r="C77" s="4"/>
+      <c r="D77" s="4"/>
+      <c r="E77" s="4"/>
+      <c r="F77" s="4"/>
+      <c r="G77" s="4"/>
+      <c r="H77" s="4"/>
+      <c r="I77" s="4"/>
+      <c r="J77" s="4"/>
+      <c r="K77" s="4"/>
+      <c r="L77" s="4"/>
     </row>
     <row r="78" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B78" s="5" t="s">
+      <c r="B78" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C78" s="5">
+      <c r="C78" s="4">
         <f>SUM(C75:L75)/10</f>
         <v>33.5</v>
       </c>
-      <c r="D78" s="5">
+      <c r="D78" s="4">
         <f>SUM(C75:L75)/10</f>
         <v>33.5</v>
       </c>
-      <c r="E78" s="5">
+      <c r="E78" s="4">
         <f>SUM(C75:L75)/10</f>
         <v>33.5</v>
       </c>
-      <c r="F78" s="5">
+      <c r="F78" s="4">
         <f>SUM(C75:L75)/10</f>
         <v>33.5</v>
       </c>
-      <c r="G78" s="5">
+      <c r="G78" s="4">
         <f>SUM(C75:L75)/10</f>
         <v>33.5</v>
       </c>
-      <c r="H78" s="5">
+      <c r="H78" s="4">
         <f>SUM(C75:L75)/10</f>
         <v>33.5</v>
       </c>
-      <c r="I78" s="5">
+      <c r="I78" s="4">
         <f>SUM(C75:L75)/10</f>
         <v>33.5</v>
       </c>
-      <c r="J78" s="5">
+      <c r="J78" s="4">
         <f>SUM(C75:L75)/10</f>
         <v>33.5</v>
       </c>
-      <c r="K78" s="5">
+      <c r="K78" s="4">
         <f>SUM(C75:L75)/10</f>
         <v>33.5</v>
       </c>
-      <c r="L78" s="5">
+      <c r="L78" s="4">
         <f>SUM(C75:L75)/10</f>
         <v>33.5</v>
       </c>
     </row>
     <row r="79" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B79" s="5" t="s">
+      <c r="B79" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C79" s="5">
+      <c r="C79" s="4">
         <f>SUM(C76:L76)/10</f>
         <v>6.4700000000000008E-2</v>
       </c>
-      <c r="D79" s="5">
+      <c r="D79" s="4">
         <f>SUM(C76:L76)/10</f>
         <v>6.4700000000000008E-2</v>
       </c>
-      <c r="E79" s="5">
+      <c r="E79" s="4">
         <f>SUM(C76:L76)/10</f>
         <v>6.4700000000000008E-2</v>
       </c>
-      <c r="F79" s="5">
+      <c r="F79" s="4">
         <f>SUM(C76:L76)/10</f>
         <v>6.4700000000000008E-2</v>
       </c>
-      <c r="G79" s="5">
+      <c r="G79" s="4">
         <f>SUM(C76:L76)/10</f>
         <v>6.4700000000000008E-2</v>
       </c>
-      <c r="H79" s="5">
+      <c r="H79" s="4">
         <f>SUM(C76:L76)/10</f>
         <v>6.4700000000000008E-2</v>
       </c>
-      <c r="I79" s="5">
+      <c r="I79" s="4">
         <f>SUM(C76:L76)/10</f>
         <v>6.4700000000000008E-2</v>
       </c>
-      <c r="J79" s="5">
+      <c r="J79" s="4">
         <f>SUM(C76:L76)/10</f>
         <v>6.4700000000000008E-2</v>
       </c>
-      <c r="K79" s="5">
+      <c r="K79" s="4">
         <f>SUM(C76:L76)/10</f>
         <v>6.4700000000000008E-2</v>
       </c>
-      <c r="L79" s="5">
+      <c r="L79" s="4">
         <f>SUM(C76:L76)/10</f>
         <v>6.4700000000000008E-2</v>
       </c>
@@ -16793,8 +16824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L43"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="P40" sqref="P40"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="V62" sqref="V62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16803,242 +16834,242 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
+      <c r="B2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>1</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>2</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>3</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <v>4</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="4">
         <v>5</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="4">
         <v>6</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="4">
         <v>7</v>
       </c>
-      <c r="J3" s="5">
+      <c r="J3" s="4">
         <v>8</v>
       </c>
-      <c r="K3" s="5">
+      <c r="K3" s="4">
         <v>9</v>
       </c>
-      <c r="L3" s="5">
+      <c r="L3" s="4">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>41</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>40</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>39</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>38</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="4">
         <v>38</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="4">
         <v>39</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="4">
         <v>39</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J4" s="4">
         <v>39</v>
       </c>
-      <c r="K4" s="5">
+      <c r="K4" s="4">
         <v>39</v>
       </c>
-      <c r="L4" s="5">
+      <c r="L4" s="4">
         <v>40</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>0.02</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>0.04</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>0.06</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>0.08</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="4">
         <v>0.08</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="4">
         <v>0.06</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="4">
         <v>0.06</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5" s="4">
         <v>0.06</v>
       </c>
-      <c r="K5" s="5">
+      <c r="K5" s="4">
         <v>0.06</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L5" s="4">
         <v>0.04</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <f>SUM(C4:L4)/10</f>
         <v>39.200000000000003</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <f>SUM(C4:L4)/10</f>
         <v>39.200000000000003</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <f>SUM(C4:L4)/10</f>
         <v>39.200000000000003</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <f>SUM(C4:L4)/10</f>
         <v>39.200000000000003</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="4">
         <f>SUM(C4:L4)/10</f>
         <v>39.200000000000003</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="4">
         <f>SUM(C4:L4)/10</f>
         <v>39.200000000000003</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="4">
         <f>SUM(C4:L4)/10</f>
         <v>39.200000000000003</v>
       </c>
-      <c r="J7" s="5">
+      <c r="J7" s="4">
         <f>SUM(C4:L4)/10</f>
         <v>39.200000000000003</v>
       </c>
-      <c r="K7" s="5">
+      <c r="K7" s="4">
         <f>SUM(C4:L4)/10</f>
         <v>39.200000000000003</v>
       </c>
-      <c r="L7" s="5">
+      <c r="L7" s="4">
         <f>SUM(C4:L4)/10</f>
         <v>39.200000000000003</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <f>SUM(C5:L5)/10</f>
         <v>5.6000000000000008E-2</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <f>SUM(C5:L5)/10</f>
         <v>5.6000000000000008E-2</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <f>SUM(C5:L5)/10</f>
         <v>5.6000000000000008E-2</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <f>SUM(C5:L5)/10</f>
         <v>5.6000000000000008E-2</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="4">
         <f>SUM(C5:L5)/10</f>
         <v>5.6000000000000008E-2</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="4">
         <f>SUM(C5:L5)/10</f>
         <v>5.6000000000000008E-2</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="4">
         <f>SUM(C5:L5)/10</f>
         <v>5.6000000000000008E-2</v>
       </c>
-      <c r="J8" s="5">
+      <c r="J8" s="4">
         <f>SUM(C5:L5)/10</f>
         <v>5.6000000000000008E-2</v>
       </c>
-      <c r="K8" s="5">
+      <c r="K8" s="4">
         <f>SUM(C5:L5)/10</f>
         <v>5.6000000000000008E-2</v>
       </c>
-      <c r="L8" s="5">
+      <c r="L8" s="4">
         <f>SUM(C5:L5)/10</f>
         <v>5.6000000000000008E-2</v>
       </c>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B37" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7"/>
-      <c r="H37" s="7"/>
-      <c r="I37" s="7"/>
-      <c r="J37" s="7"/>
-      <c r="K37" s="7"/>
-      <c r="L37" s="7"/>
+      <c r="B37" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="9"/>
+      <c r="J37" s="9"/>
+      <c r="K37" s="9"/>
+      <c r="L37" s="9"/>
     </row>
     <row r="38" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
@@ -17272,409 +17303,452 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:W8"/>
+  <dimension ref="C1:W8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="Z17" sqref="Z17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="2.85546875" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="4" max="5" width="10.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" customWidth="1"/>
+    <col min="9" max="11" width="9.5703125" customWidth="1"/>
+    <col min="12" max="12" width="9.85546875" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" customWidth="1"/>
+    <col min="14" max="14" width="10.28515625" customWidth="1"/>
+    <col min="15" max="15" width="10.42578125" customWidth="1"/>
+    <col min="16" max="16" width="10.28515625" customWidth="1"/>
+    <col min="17" max="18" width="10.42578125" customWidth="1"/>
+    <col min="19" max="20" width="10.85546875" customWidth="1"/>
+    <col min="21" max="21" width="10.28515625" customWidth="1"/>
+    <col min="22" max="23" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C1" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+    </row>
     <row r="2" spans="3:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="4"/>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="R2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="S2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="T2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="U2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="V2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="W2" s="4" t="s">
-        <v>10</v>
+      <c r="R2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="3:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>41</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>38</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>38</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="3">
         <v>38</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="3">
         <v>39</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="3">
         <v>37</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3" s="3">
         <v>38</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K3" s="3">
         <v>37</v>
       </c>
-      <c r="L3" s="4">
+      <c r="L3" s="3">
         <v>36</v>
       </c>
-      <c r="M3" s="4">
+      <c r="M3" s="3">
         <v>36</v>
       </c>
-      <c r="N3" s="4">
+      <c r="N3" s="3">
         <v>35</v>
       </c>
-      <c r="O3" s="4">
+      <c r="O3" s="3">
         <v>36</v>
       </c>
-      <c r="P3" s="4">
+      <c r="P3" s="3">
         <v>35</v>
       </c>
-      <c r="Q3" s="4">
+      <c r="Q3" s="3">
         <v>36</v>
       </c>
-      <c r="R3" s="4">
+      <c r="R3" s="3">
         <v>35</v>
       </c>
-      <c r="S3" s="4">
+      <c r="S3" s="3">
         <v>34</v>
       </c>
-      <c r="T3" s="4">
+      <c r="T3" s="3">
         <v>34</v>
       </c>
-      <c r="U3" s="4">
+      <c r="U3" s="3">
         <v>34</v>
       </c>
-      <c r="V3" s="4">
+      <c r="V3" s="3">
         <v>34</v>
       </c>
-      <c r="W3" s="4">
+      <c r="W3" s="3">
         <v>35</v>
       </c>
     </row>
     <row r="4" spans="3:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>40</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>37</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>37</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <v>38</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="3">
         <v>37</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="3">
         <v>35</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="3">
         <v>34</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4" s="3">
         <v>33</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4" s="3">
         <v>33</v>
       </c>
-      <c r="M4" s="4">
+      <c r="M4" s="3">
         <v>31</v>
       </c>
-      <c r="N4" s="4">
+      <c r="N4" s="3">
         <v>32</v>
       </c>
-      <c r="O4" s="4">
+      <c r="O4" s="3">
         <v>31</v>
       </c>
-      <c r="P4" s="4">
+      <c r="P4" s="3">
         <v>31</v>
       </c>
-      <c r="Q4" s="4">
+      <c r="Q4" s="3">
         <v>30</v>
       </c>
-      <c r="R4" s="4">
+      <c r="R4" s="3">
         <v>30</v>
       </c>
-      <c r="S4" s="4">
+      <c r="S4" s="3">
         <v>31</v>
       </c>
-      <c r="T4" s="4">
+      <c r="T4" s="3">
         <v>32</v>
       </c>
-      <c r="U4" s="4">
+      <c r="U4" s="3">
         <v>31</v>
       </c>
-      <c r="V4" s="4">
+      <c r="V4" s="3">
         <v>30</v>
       </c>
-      <c r="W4" s="4">
+      <c r="W4" s="3">
         <v>32</v>
       </c>
     </row>
     <row r="5" spans="3:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>44</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>44</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <v>41</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <v>37</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="3">
         <v>37</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="3">
         <v>36</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5" s="3">
         <v>38</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5" s="3">
         <v>37</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L5" s="3">
         <v>36</v>
       </c>
-      <c r="M5" s="4">
+      <c r="M5" s="3">
         <v>37</v>
       </c>
-      <c r="N5" s="4">
+      <c r="N5" s="3">
         <v>37</v>
       </c>
-      <c r="O5" s="4">
+      <c r="O5" s="3">
         <v>37</v>
       </c>
-      <c r="P5" s="4">
+      <c r="P5" s="3">
         <v>35</v>
       </c>
-      <c r="Q5" s="4">
+      <c r="Q5" s="3">
         <v>33</v>
       </c>
-      <c r="R5" s="4">
+      <c r="R5" s="3">
         <v>34</v>
       </c>
-      <c r="S5" s="4">
+      <c r="S5" s="3">
         <v>35</v>
       </c>
-      <c r="T5" s="4">
+      <c r="T5" s="3">
         <v>33</v>
       </c>
-      <c r="U5" s="4">
+      <c r="U5" s="3">
         <v>33</v>
       </c>
-      <c r="V5" s="4">
+      <c r="V5" s="3">
         <v>31</v>
       </c>
-      <c r="W5" s="4">
+      <c r="W5" s="3">
         <v>31</v>
       </c>
     </row>
     <row r="6" spans="3:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>40</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>40</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>40</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="3">
         <v>39</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="3">
         <v>38</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="3">
         <v>39</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6" s="3">
         <v>38</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6" s="3">
         <v>39</v>
       </c>
-      <c r="L6" s="4">
+      <c r="L6" s="3">
         <v>40</v>
       </c>
-      <c r="M6" s="4">
+      <c r="M6" s="3">
         <v>40</v>
       </c>
-      <c r="N6" s="4">
+      <c r="N6" s="3">
         <v>38</v>
       </c>
-      <c r="O6" s="4">
+      <c r="O6" s="3">
         <v>38</v>
       </c>
-      <c r="P6" s="4">
+      <c r="P6" s="3">
         <v>38</v>
       </c>
-      <c r="Q6" s="4">
+      <c r="Q6" s="3">
         <v>38</v>
       </c>
-      <c r="R6" s="4">
+      <c r="R6" s="3">
         <v>38</v>
       </c>
-      <c r="S6" s="4">
+      <c r="S6" s="3">
         <v>37</v>
       </c>
-      <c r="T6" s="4">
+      <c r="T6" s="3">
         <v>38</v>
       </c>
-      <c r="U6" s="4">
+      <c r="U6" s="3">
         <v>37</v>
       </c>
-      <c r="V6" s="4">
+      <c r="V6" s="3">
         <v>37</v>
       </c>
-      <c r="W6" s="4">
+      <c r="W6" s="3">
         <v>37</v>
       </c>
     </row>
     <row r="7" spans="3:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>44</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>43</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="3">
         <v>42</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="3">
         <v>41</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="3">
         <v>41</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="3">
         <v>40</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J7" s="3">
         <v>38</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K7" s="3">
         <v>39</v>
       </c>
-      <c r="L7" s="4">
+      <c r="L7" s="3">
         <v>39</v>
       </c>
-      <c r="M7" s="4">
+      <c r="M7" s="3">
         <v>36</v>
       </c>
-      <c r="N7" s="4">
+      <c r="N7" s="3">
         <v>36</v>
       </c>
-      <c r="O7" s="4">
+      <c r="O7" s="3">
         <v>37</v>
       </c>
-      <c r="P7" s="4">
+      <c r="P7" s="3">
         <v>38</v>
       </c>
-      <c r="Q7" s="4">
+      <c r="Q7" s="3">
         <v>40</v>
       </c>
-      <c r="R7" s="4">
+      <c r="R7" s="3">
         <v>40</v>
       </c>
-      <c r="S7" s="4">
+      <c r="S7" s="3">
         <v>40</v>
       </c>
-      <c r="T7" s="4">
+      <c r="T7" s="3">
         <v>41</v>
       </c>
-      <c r="U7" s="4">
+      <c r="U7" s="3">
         <v>38</v>
       </c>
-      <c r="V7" s="4">
+      <c r="V7" s="3">
         <v>35</v>
       </c>
-      <c r="W7" s="4">
+      <c r="W7" s="3">
         <v>34</v>
       </c>
     </row>
     <row r="8" spans="3:23" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:G1"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>